<commit_message>
add tblVendState excel sheet
</commit_message>
<xml_diff>
--- a/UT.Vend.BLL/HelperFiles/tblVendState.xlsx
+++ b/UT.Vend.BLL/HelperFiles/tblVendState.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="73">
   <si>
     <t>StateID</t>
   </si>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t>Query</t>
+  </si>
+  <si>
+    <t>Volteer.Vend.tblVendState</t>
   </si>
 </sst>
 </file>
@@ -559,7 +562,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AK2" sqref="AK2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -571,7 +576,7 @@
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="22" bestFit="1" customWidth="1"/>
@@ -582,6 +587,9 @@
       <c r="A1" t="s">
         <v>62</v>
       </c>
+      <c r="M1" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -688,6 +696,10 @@
       <c r="Q3">
         <v>3</v>
       </c>
+      <c r="R3" t="str">
+        <f>"INSERT INTO Volteer.Vend.tblVendState (["&amp;M$2&amp;"],["&amp;N$2&amp;"],["&amp;O$2&amp;"],["&amp;P$2&amp;"],["&amp;Q$2&amp;"]) VALUES ('"&amp;M3&amp;"', '"&amp;N3&amp;"', '"&amp;O3&amp;"', '"&amp;P3&amp;"', '"&amp;Q3&amp;"')"</f>
+        <v>INSERT INTO Volteer.Vend.tblVendState ([census_region],[census_region_name],[census_division],[census_devision_name],[circuit_court]) VALUES ('3', 'South', '5', 'South Atlantic', '3')</v>
+      </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -738,6 +750,10 @@
       <c r="Q4">
         <v>8</v>
       </c>
+      <c r="R4" t="str">
+        <f t="shared" ref="R4:R12" si="0">"INSERT INTO Volteer.Vend.tblVendState (["&amp;M$2&amp;"],["&amp;N$2&amp;"],["&amp;O$2&amp;"],["&amp;P$2&amp;"],["&amp;Q$2&amp;"]) VALUES ('"&amp;M4&amp;"', '"&amp;N4&amp;"', '"&amp;O4&amp;"', '"&amp;P4&amp;"', '"&amp;Q4&amp;"')"</f>
+        <v>INSERT INTO Volteer.Vend.tblVendState ([census_region],[census_region_name],[census_division],[census_devision_name],[circuit_court]) VALUES ('2', 'Midwest', '4', 'West North Central', '8')</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -788,6 +804,10 @@
       <c r="Q5">
         <v>9</v>
       </c>
+      <c r="R5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Volteer.Vend.tblVendState ([census_region],[census_region_name],[census_division],[census_devision_name],[circuit_court]) VALUES ('4', 'West', '9', 'Pacfic', '9')</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -838,6 +858,10 @@
       <c r="Q6">
         <v>3</v>
       </c>
+      <c r="R6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Volteer.Vend.tblVendState ([census_region],[census_region_name],[census_division],[census_devision_name],[circuit_court]) VALUES ('1', 'Northeast', '2', 'Mid-Atlantic', '3')</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -888,6 +912,10 @@
       <c r="Q7">
         <v>9</v>
       </c>
+      <c r="R7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Volteer.Vend.tblVendState ([census_region],[census_region_name],[census_division],[census_devision_name],[circuit_court]) VALUES ('4', 'West', '9', 'Pacfic', '9')</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -938,6 +966,10 @@
       <c r="Q8">
         <v>11</v>
       </c>
+      <c r="R8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Volteer.Vend.tblVendState ([census_region],[census_region_name],[census_division],[census_devision_name],[circuit_court]) VALUES ('3', 'South', '6', 'East South Central', '11')</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -988,6 +1020,10 @@
       <c r="Q9">
         <v>10</v>
       </c>
+      <c r="R9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Volteer.Vend.tblVendState ([census_region],[census_region_name],[census_division],[census_devision_name],[circuit_court]) VALUES ('4', 'West', '8', 'Mountain', '10')</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1038,6 +1074,10 @@
       <c r="Q10">
         <v>9</v>
       </c>
+      <c r="R10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Volteer.Vend.tblVendState ([census_region],[census_region_name],[census_division],[census_devision_name],[circuit_court]) VALUES ('4', 'West', '9', 'Pacfic', '9')</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1088,6 +1128,10 @@
       <c r="Q11">
         <v>7</v>
       </c>
+      <c r="R11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Volteer.Vend.tblVendState ([census_region],[census_region_name],[census_division],[census_devision_name],[circuit_court]) VALUES ('2', 'Midwest', '3', 'East North Central', '7')</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1137,6 +1181,10 @@
       </c>
       <c r="Q12">
         <v>3</v>
+      </c>
+      <c r="R12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Volteer.Vend.tblVendState ([census_region],[census_region_name],[census_division],[census_devision_name],[circuit_court]) VALUES ('3', 'FarEast', '3', 'East', '3')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>